<commit_message>
Updated database files and added sql for whole database structure
</commit_message>
<xml_diff>
--- a/database_files/TestData.xlsx
+++ b/database_files/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03BDC9A4-EAA1-495D-B4F9-F511DC8E5B1F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{91E0B686-4D20-4B2E-BCFC-6371A17C7F53}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="328">
   <si>
     <t>team 1</t>
   </si>
@@ -944,6 +944,72 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>AT1</t>
+  </si>
+  <si>
+    <t>AT2</t>
+  </si>
+  <si>
+    <t>AT3</t>
+  </si>
+  <si>
+    <t>AT4</t>
+  </si>
+  <si>
+    <t>AT5</t>
+  </si>
+  <si>
+    <t>AT6</t>
+  </si>
+  <si>
+    <t>AT7</t>
+  </si>
+  <si>
+    <t>AT8</t>
+  </si>
+  <si>
+    <t>AT9</t>
+  </si>
+  <si>
+    <t>AT10</t>
+  </si>
+  <si>
+    <t>AT11</t>
+  </si>
+  <si>
+    <t>AT12</t>
+  </si>
+  <si>
+    <t>AT13</t>
+  </si>
+  <si>
+    <t>AT14</t>
+  </si>
+  <si>
+    <t>AT15</t>
+  </si>
+  <si>
+    <t>AT16</t>
+  </si>
+  <si>
+    <t>AT17</t>
+  </si>
+  <si>
+    <t>AT18</t>
+  </si>
+  <si>
+    <t>AT19</t>
+  </si>
+  <si>
+    <t>AT20</t>
+  </si>
+  <si>
+    <t>ST1</t>
+  </si>
+  <si>
+    <t>ST2</t>
   </si>
 </sst>
 </file>
@@ -1264,8 +1330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
-      <selection activeCell="H298" sqref="H298"/>
+    <sheetView tabSelected="1" topLeftCell="A283" workbookViewId="0">
+      <selection activeCell="D301" sqref="D301:D308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,7 +1351,7 @@
         <v>305</v>
       </c>
       <c r="D1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1299,7 +1365,7 @@
         <v>305</v>
       </c>
       <c r="D2" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1313,7 +1379,7 @@
         <v>305</v>
       </c>
       <c r="D3" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1327,7 +1393,7 @@
         <v>305</v>
       </c>
       <c r="D4" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1341,7 +1407,7 @@
         <v>305</v>
       </c>
       <c r="D5" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1355,7 +1421,7 @@
         <v>305</v>
       </c>
       <c r="D6" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1369,7 +1435,7 @@
         <v>305</v>
       </c>
       <c r="D7" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1383,7 +1449,7 @@
         <v>305</v>
       </c>
       <c r="D8" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1397,7 +1463,7 @@
         <v>305</v>
       </c>
       <c r="D9" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1411,7 +1477,7 @@
         <v>305</v>
       </c>
       <c r="D10" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1425,7 +1491,7 @@
         <v>305</v>
       </c>
       <c r="D11" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1439,7 +1505,7 @@
         <v>305</v>
       </c>
       <c r="D12" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1453,7 +1519,7 @@
         <v>305</v>
       </c>
       <c r="D13" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1467,7 +1533,7 @@
         <v>305</v>
       </c>
       <c r="D14" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1481,7 +1547,7 @@
         <v>305</v>
       </c>
       <c r="D15" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1495,7 +1561,7 @@
         <v>305</v>
       </c>
       <c r="D16" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1509,7 +1575,7 @@
         <v>305</v>
       </c>
       <c r="D17" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1523,7 +1589,7 @@
         <v>305</v>
       </c>
       <c r="D18" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1537,7 +1603,7 @@
         <v>305</v>
       </c>
       <c r="D19" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1551,7 +1617,7 @@
         <v>305</v>
       </c>
       <c r="D20" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1565,7 +1631,7 @@
         <v>305</v>
       </c>
       <c r="D21" t="s">
-        <v>305</v>
+        <v>326</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1579,7 +1645,7 @@
         <v>305</v>
       </c>
       <c r="D22" t="s">
-        <v>305</v>
+        <v>327</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1593,7 +1659,7 @@
         <v>305</v>
       </c>
       <c r="D23" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1607,7 +1673,7 @@
         <v>305</v>
       </c>
       <c r="D24" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1621,7 +1687,7 @@
         <v>305</v>
       </c>
       <c r="D25" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1635,7 +1701,7 @@
         <v>305</v>
       </c>
       <c r="D26" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1649,7 +1715,7 @@
         <v>305</v>
       </c>
       <c r="D27" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1663,7 +1729,7 @@
         <v>305</v>
       </c>
       <c r="D28" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1677,7 +1743,7 @@
         <v>305</v>
       </c>
       <c r="D29" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1691,7 +1757,7 @@
         <v>305</v>
       </c>
       <c r="D30" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1705,7 +1771,7 @@
         <v>305</v>
       </c>
       <c r="D31" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1719,7 +1785,7 @@
         <v>305</v>
       </c>
       <c r="D32" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1733,7 +1799,7 @@
         <v>305</v>
       </c>
       <c r="D33" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1747,7 +1813,7 @@
         <v>305</v>
       </c>
       <c r="D34" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1761,7 +1827,7 @@
         <v>305</v>
       </c>
       <c r="D35" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1775,7 +1841,7 @@
         <v>305</v>
       </c>
       <c r="D36" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1789,7 +1855,7 @@
         <v>305</v>
       </c>
       <c r="D37" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1803,7 +1869,7 @@
         <v>305</v>
       </c>
       <c r="D38" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1817,7 +1883,7 @@
         <v>305</v>
       </c>
       <c r="D39" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1831,7 +1897,7 @@
         <v>305</v>
       </c>
       <c r="D40" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1845,7 +1911,7 @@
         <v>305</v>
       </c>
       <c r="D41" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1859,7 +1925,7 @@
         <v>305</v>
       </c>
       <c r="D42" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1873,7 +1939,7 @@
         <v>305</v>
       </c>
       <c r="D43" t="s">
-        <v>305</v>
+        <v>326</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1887,7 +1953,7 @@
         <v>305</v>
       </c>
       <c r="D44" t="s">
-        <v>305</v>
+        <v>327</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1901,7 +1967,7 @@
         <v>305</v>
       </c>
       <c r="D45" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1915,7 +1981,7 @@
         <v>305</v>
       </c>
       <c r="D46" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1929,7 +1995,7 @@
         <v>305</v>
       </c>
       <c r="D47" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1943,7 +2009,7 @@
         <v>305</v>
       </c>
       <c r="D48" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1957,7 +2023,7 @@
         <v>305</v>
       </c>
       <c r="D49" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1971,7 +2037,7 @@
         <v>305</v>
       </c>
       <c r="D50" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1985,7 +2051,7 @@
         <v>305</v>
       </c>
       <c r="D51" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1999,7 +2065,7 @@
         <v>305</v>
       </c>
       <c r="D52" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2013,7 +2079,7 @@
         <v>305</v>
       </c>
       <c r="D53" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2027,7 +2093,7 @@
         <v>305</v>
       </c>
       <c r="D54" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2041,7 +2107,7 @@
         <v>305</v>
       </c>
       <c r="D55" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2055,7 +2121,7 @@
         <v>305</v>
       </c>
       <c r="D56" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2069,7 +2135,7 @@
         <v>305</v>
       </c>
       <c r="D57" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2083,7 +2149,7 @@
         <v>305</v>
       </c>
       <c r="D58" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2097,7 +2163,7 @@
         <v>305</v>
       </c>
       <c r="D59" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2111,7 +2177,7 @@
         <v>305</v>
       </c>
       <c r="D60" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2125,7 +2191,7 @@
         <v>305</v>
       </c>
       <c r="D61" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2139,7 +2205,7 @@
         <v>305</v>
       </c>
       <c r="D62" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2153,7 +2219,7 @@
         <v>305</v>
       </c>
       <c r="D63" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2167,7 +2233,7 @@
         <v>305</v>
       </c>
       <c r="D64" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2181,7 +2247,7 @@
         <v>305</v>
       </c>
       <c r="D65" t="s">
-        <v>305</v>
+        <v>326</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2195,7 +2261,7 @@
         <v>305</v>
       </c>
       <c r="D66" t="s">
-        <v>305</v>
+        <v>327</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2209,7 +2275,7 @@
         <v>305</v>
       </c>
       <c r="D67" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2223,7 +2289,7 @@
         <v>305</v>
       </c>
       <c r="D68" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2237,7 +2303,7 @@
         <v>305</v>
       </c>
       <c r="D69" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2251,7 +2317,7 @@
         <v>305</v>
       </c>
       <c r="D70" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2265,7 +2331,7 @@
         <v>305</v>
       </c>
       <c r="D71" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2279,7 +2345,7 @@
         <v>305</v>
       </c>
       <c r="D72" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2293,7 +2359,7 @@
         <v>305</v>
       </c>
       <c r="D73" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2307,7 +2373,7 @@
         <v>305</v>
       </c>
       <c r="D74" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2321,7 +2387,7 @@
         <v>305</v>
       </c>
       <c r="D75" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2335,7 +2401,7 @@
         <v>305</v>
       </c>
       <c r="D76" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2349,7 +2415,7 @@
         <v>305</v>
       </c>
       <c r="D77" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2363,7 +2429,7 @@
         <v>305</v>
       </c>
       <c r="D78" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2377,7 +2443,7 @@
         <v>305</v>
       </c>
       <c r="D79" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2391,7 +2457,7 @@
         <v>305</v>
       </c>
       <c r="D80" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2405,7 +2471,7 @@
         <v>305</v>
       </c>
       <c r="D81" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2419,7 +2485,7 @@
         <v>305</v>
       </c>
       <c r="D82" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2433,7 +2499,7 @@
         <v>305</v>
       </c>
       <c r="D83" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2447,7 +2513,7 @@
         <v>305</v>
       </c>
       <c r="D84" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2461,7 +2527,7 @@
         <v>305</v>
       </c>
       <c r="D85" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2475,7 +2541,7 @@
         <v>305</v>
       </c>
       <c r="D86" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2489,7 +2555,7 @@
         <v>305</v>
       </c>
       <c r="D87" t="s">
-        <v>305</v>
+        <v>326</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2503,7 +2569,7 @@
         <v>305</v>
       </c>
       <c r="D88" t="s">
-        <v>305</v>
+        <v>327</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2517,7 +2583,7 @@
         <v>305</v>
       </c>
       <c r="D89" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2531,7 +2597,7 @@
         <v>305</v>
       </c>
       <c r="D90" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2545,7 +2611,7 @@
         <v>305</v>
       </c>
       <c r="D91" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2559,7 +2625,7 @@
         <v>305</v>
       </c>
       <c r="D92" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2573,7 +2639,7 @@
         <v>305</v>
       </c>
       <c r="D93" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2587,7 +2653,7 @@
         <v>305</v>
       </c>
       <c r="D94" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2601,7 +2667,7 @@
         <v>305</v>
       </c>
       <c r="D95" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2615,7 +2681,7 @@
         <v>305</v>
       </c>
       <c r="D96" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2629,7 +2695,7 @@
         <v>305</v>
       </c>
       <c r="D97" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2643,7 +2709,7 @@
         <v>305</v>
       </c>
       <c r="D98" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2657,7 +2723,7 @@
         <v>305</v>
       </c>
       <c r="D99" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2671,7 +2737,7 @@
         <v>305</v>
       </c>
       <c r="D100" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2685,7 +2751,7 @@
         <v>305</v>
       </c>
       <c r="D101" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2699,7 +2765,7 @@
         <v>305</v>
       </c>
       <c r="D102" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2713,7 +2779,7 @@
         <v>305</v>
       </c>
       <c r="D103" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2727,7 +2793,7 @@
         <v>305</v>
       </c>
       <c r="D104" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2741,7 +2807,7 @@
         <v>305</v>
       </c>
       <c r="D105" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -2755,7 +2821,7 @@
         <v>305</v>
       </c>
       <c r="D106" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2769,7 +2835,7 @@
         <v>305</v>
       </c>
       <c r="D107" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2783,7 +2849,7 @@
         <v>305</v>
       </c>
       <c r="D108" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2797,7 +2863,7 @@
         <v>305</v>
       </c>
       <c r="D109" t="s">
-        <v>305</v>
+        <v>326</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -2811,7 +2877,7 @@
         <v>305</v>
       </c>
       <c r="D110" t="s">
-        <v>305</v>
+        <v>327</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2825,7 +2891,7 @@
         <v>305</v>
       </c>
       <c r="D111" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -2839,7 +2905,7 @@
         <v>305</v>
       </c>
       <c r="D112" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -2853,7 +2919,7 @@
         <v>305</v>
       </c>
       <c r="D113" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -2867,7 +2933,7 @@
         <v>305</v>
       </c>
       <c r="D114" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -2881,7 +2947,7 @@
         <v>305</v>
       </c>
       <c r="D115" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -2895,7 +2961,7 @@
         <v>305</v>
       </c>
       <c r="D116" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -2909,7 +2975,7 @@
         <v>305</v>
       </c>
       <c r="D117" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -2923,7 +2989,7 @@
         <v>305</v>
       </c>
       <c r="D118" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -2937,7 +3003,7 @@
         <v>305</v>
       </c>
       <c r="D119" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -2951,7 +3017,7 @@
         <v>305</v>
       </c>
       <c r="D120" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -2965,7 +3031,7 @@
         <v>305</v>
       </c>
       <c r="D121" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -2979,7 +3045,7 @@
         <v>305</v>
       </c>
       <c r="D122" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -2993,7 +3059,7 @@
         <v>305</v>
       </c>
       <c r="D123" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3007,7 +3073,7 @@
         <v>305</v>
       </c>
       <c r="D124" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3021,7 +3087,7 @@
         <v>305</v>
       </c>
       <c r="D125" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3035,7 +3101,7 @@
         <v>305</v>
       </c>
       <c r="D126" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -3049,7 +3115,7 @@
         <v>305</v>
       </c>
       <c r="D127" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -3063,7 +3129,7 @@
         <v>305</v>
       </c>
       <c r="D128" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3077,7 +3143,7 @@
         <v>305</v>
       </c>
       <c r="D129" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -3091,7 +3157,7 @@
         <v>305</v>
       </c>
       <c r="D130" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3105,7 +3171,7 @@
         <v>305</v>
       </c>
       <c r="D131" t="s">
-        <v>305</v>
+        <v>326</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3119,7 +3185,7 @@
         <v>305</v>
       </c>
       <c r="D132" t="s">
-        <v>305</v>
+        <v>327</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -3133,7 +3199,7 @@
         <v>305</v>
       </c>
       <c r="D133" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -3147,7 +3213,7 @@
         <v>305</v>
       </c>
       <c r="D134" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -3161,7 +3227,7 @@
         <v>305</v>
       </c>
       <c r="D135" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -3175,7 +3241,7 @@
         <v>305</v>
       </c>
       <c r="D136" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -3189,7 +3255,7 @@
         <v>305</v>
       </c>
       <c r="D137" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -3203,7 +3269,7 @@
         <v>305</v>
       </c>
       <c r="D138" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -3217,7 +3283,7 @@
         <v>305</v>
       </c>
       <c r="D139" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -3231,7 +3297,7 @@
         <v>305</v>
       </c>
       <c r="D140" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -3245,7 +3311,7 @@
         <v>305</v>
       </c>
       <c r="D141" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -3259,7 +3325,7 @@
         <v>305</v>
       </c>
       <c r="D142" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -3273,7 +3339,7 @@
         <v>305</v>
       </c>
       <c r="D143" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -3287,7 +3353,7 @@
         <v>305</v>
       </c>
       <c r="D144" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -3301,7 +3367,7 @@
         <v>305</v>
       </c>
       <c r="D145" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -3315,7 +3381,7 @@
         <v>305</v>
       </c>
       <c r="D146" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -3329,7 +3395,7 @@
         <v>305</v>
       </c>
       <c r="D147" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -3343,7 +3409,7 @@
         <v>305</v>
       </c>
       <c r="D148" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -3357,7 +3423,7 @@
         <v>305</v>
       </c>
       <c r="D149" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -3371,7 +3437,7 @@
         <v>305</v>
       </c>
       <c r="D150" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -3385,7 +3451,7 @@
         <v>305</v>
       </c>
       <c r="D151" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -3399,7 +3465,7 @@
         <v>305</v>
       </c>
       <c r="D152" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -3413,7 +3479,7 @@
         <v>305</v>
       </c>
       <c r="D153" t="s">
-        <v>305</v>
+        <v>326</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -3427,7 +3493,7 @@
         <v>305</v>
       </c>
       <c r="D154" t="s">
-        <v>305</v>
+        <v>327</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -3441,7 +3507,7 @@
         <v>305</v>
       </c>
       <c r="D155" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -3455,7 +3521,7 @@
         <v>305</v>
       </c>
       <c r="D156" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -3469,7 +3535,7 @@
         <v>305</v>
       </c>
       <c r="D157" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -3483,7 +3549,7 @@
         <v>305</v>
       </c>
       <c r="D158" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -3497,7 +3563,7 @@
         <v>305</v>
       </c>
       <c r="D159" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -3511,7 +3577,7 @@
         <v>305</v>
       </c>
       <c r="D160" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -3525,7 +3591,7 @@
         <v>305</v>
       </c>
       <c r="D161" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -3539,7 +3605,7 @@
         <v>305</v>
       </c>
       <c r="D162" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -3553,7 +3619,7 @@
         <v>305</v>
       </c>
       <c r="D163" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -3567,7 +3633,7 @@
         <v>305</v>
       </c>
       <c r="D164" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -3581,7 +3647,7 @@
         <v>305</v>
       </c>
       <c r="D165" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -3595,7 +3661,7 @@
         <v>305</v>
       </c>
       <c r="D166" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -3609,7 +3675,7 @@
         <v>305</v>
       </c>
       <c r="D167" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -3623,7 +3689,7 @@
         <v>305</v>
       </c>
       <c r="D168" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -3637,7 +3703,7 @@
         <v>305</v>
       </c>
       <c r="D169" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -3651,7 +3717,7 @@
         <v>305</v>
       </c>
       <c r="D170" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -3665,7 +3731,7 @@
         <v>305</v>
       </c>
       <c r="D171" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -3679,7 +3745,7 @@
         <v>305</v>
       </c>
       <c r="D172" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -3693,7 +3759,7 @@
         <v>305</v>
       </c>
       <c r="D173" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -3707,7 +3773,7 @@
         <v>305</v>
       </c>
       <c r="D174" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -3721,7 +3787,7 @@
         <v>305</v>
       </c>
       <c r="D175" t="s">
-        <v>305</v>
+        <v>326</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -3735,7 +3801,7 @@
         <v>305</v>
       </c>
       <c r="D176" t="s">
-        <v>305</v>
+        <v>327</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -3749,7 +3815,7 @@
         <v>305</v>
       </c>
       <c r="D177" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -3763,7 +3829,7 @@
         <v>305</v>
       </c>
       <c r="D178" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -3777,7 +3843,7 @@
         <v>305</v>
       </c>
       <c r="D179" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -3791,7 +3857,7 @@
         <v>305</v>
       </c>
       <c r="D180" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -3805,7 +3871,7 @@
         <v>305</v>
       </c>
       <c r="D181" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -3819,7 +3885,7 @@
         <v>305</v>
       </c>
       <c r="D182" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -3833,7 +3899,7 @@
         <v>305</v>
       </c>
       <c r="D183" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -3847,7 +3913,7 @@
         <v>305</v>
       </c>
       <c r="D184" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -3861,7 +3927,7 @@
         <v>305</v>
       </c>
       <c r="D185" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -3875,7 +3941,7 @@
         <v>305</v>
       </c>
       <c r="D186" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -3889,7 +3955,7 @@
         <v>305</v>
       </c>
       <c r="D187" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -3903,7 +3969,7 @@
         <v>305</v>
       </c>
       <c r="D188" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -3917,7 +3983,7 @@
         <v>305</v>
       </c>
       <c r="D189" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -3931,7 +3997,7 @@
         <v>305</v>
       </c>
       <c r="D190" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -3945,7 +4011,7 @@
         <v>305</v>
       </c>
       <c r="D191" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -3959,7 +4025,7 @@
         <v>305</v>
       </c>
       <c r="D192" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -3973,7 +4039,7 @@
         <v>305</v>
       </c>
       <c r="D193" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -3987,7 +4053,7 @@
         <v>305</v>
       </c>
       <c r="D194" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -4001,7 +4067,7 @@
         <v>305</v>
       </c>
       <c r="D195" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -4015,7 +4081,7 @@
         <v>305</v>
       </c>
       <c r="D196" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -4029,7 +4095,7 @@
         <v>305</v>
       </c>
       <c r="D197" t="s">
-        <v>305</v>
+        <v>326</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -4043,7 +4109,7 @@
         <v>305</v>
       </c>
       <c r="D198" t="s">
-        <v>305</v>
+        <v>327</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -4057,7 +4123,7 @@
         <v>305</v>
       </c>
       <c r="D199" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -4071,7 +4137,7 @@
         <v>305</v>
       </c>
       <c r="D200" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -4085,7 +4151,7 @@
         <v>305</v>
       </c>
       <c r="D201" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -4099,7 +4165,7 @@
         <v>305</v>
       </c>
       <c r="D202" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -4113,7 +4179,7 @@
         <v>305</v>
       </c>
       <c r="D203" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -4127,7 +4193,7 @@
         <v>305</v>
       </c>
       <c r="D204" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -4141,7 +4207,7 @@
         <v>305</v>
       </c>
       <c r="D205" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -4155,7 +4221,7 @@
         <v>305</v>
       </c>
       <c r="D206" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -4169,7 +4235,7 @@
         <v>305</v>
       </c>
       <c r="D207" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -4183,7 +4249,7 @@
         <v>305</v>
       </c>
       <c r="D208" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -4197,7 +4263,7 @@
         <v>305</v>
       </c>
       <c r="D209" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -4211,7 +4277,7 @@
         <v>305</v>
       </c>
       <c r="D210" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -4225,7 +4291,7 @@
         <v>305</v>
       </c>
       <c r="D211" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -4239,7 +4305,7 @@
         <v>305</v>
       </c>
       <c r="D212" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -4253,7 +4319,7 @@
         <v>305</v>
       </c>
       <c r="D213" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -4267,7 +4333,7 @@
         <v>305</v>
       </c>
       <c r="D214" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -4281,7 +4347,7 @@
         <v>305</v>
       </c>
       <c r="D215" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -4295,7 +4361,7 @@
         <v>305</v>
       </c>
       <c r="D216" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -4309,7 +4375,7 @@
         <v>305</v>
       </c>
       <c r="D217" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -4323,7 +4389,7 @@
         <v>305</v>
       </c>
       <c r="D218" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -4337,7 +4403,7 @@
         <v>305</v>
       </c>
       <c r="D219" t="s">
-        <v>305</v>
+        <v>326</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -4351,7 +4417,7 @@
         <v>305</v>
       </c>
       <c r="D220" t="s">
-        <v>305</v>
+        <v>327</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -4365,7 +4431,7 @@
         <v>305</v>
       </c>
       <c r="D221" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -4379,7 +4445,7 @@
         <v>305</v>
       </c>
       <c r="D222" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -4393,7 +4459,7 @@
         <v>305</v>
       </c>
       <c r="D223" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -4407,7 +4473,7 @@
         <v>305</v>
       </c>
       <c r="D224" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -4421,7 +4487,7 @@
         <v>305</v>
       </c>
       <c r="D225" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -4435,7 +4501,7 @@
         <v>305</v>
       </c>
       <c r="D226" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
@@ -4449,7 +4515,7 @@
         <v>305</v>
       </c>
       <c r="D227" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -4463,7 +4529,7 @@
         <v>305</v>
       </c>
       <c r="D228" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
@@ -4477,7 +4543,7 @@
         <v>305</v>
       </c>
       <c r="D229" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
@@ -4491,7 +4557,7 @@
         <v>305</v>
       </c>
       <c r="D230" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
@@ -4505,7 +4571,7 @@
         <v>305</v>
       </c>
       <c r="D231" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
@@ -4519,7 +4585,7 @@
         <v>305</v>
       </c>
       <c r="D232" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
@@ -4533,7 +4599,7 @@
         <v>305</v>
       </c>
       <c r="D233" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -4547,7 +4613,7 @@
         <v>305</v>
       </c>
       <c r="D234" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
@@ -4561,7 +4627,7 @@
         <v>305</v>
       </c>
       <c r="D235" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
@@ -4575,7 +4641,7 @@
         <v>305</v>
       </c>
       <c r="D236" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -4589,7 +4655,7 @@
         <v>305</v>
       </c>
       <c r="D237" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
@@ -4603,7 +4669,7 @@
         <v>305</v>
       </c>
       <c r="D238" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
@@ -4617,7 +4683,7 @@
         <v>305</v>
       </c>
       <c r="D239" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
@@ -4631,7 +4697,7 @@
         <v>305</v>
       </c>
       <c r="D240" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -4645,7 +4711,7 @@
         <v>305</v>
       </c>
       <c r="D241" t="s">
-        <v>305</v>
+        <v>326</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -4659,7 +4725,7 @@
         <v>305</v>
       </c>
       <c r="D242" t="s">
-        <v>305</v>
+        <v>327</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
@@ -4673,7 +4739,7 @@
         <v>305</v>
       </c>
       <c r="D243" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
@@ -4687,7 +4753,7 @@
         <v>305</v>
       </c>
       <c r="D244" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
@@ -4701,7 +4767,7 @@
         <v>305</v>
       </c>
       <c r="D245" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
@@ -4715,7 +4781,7 @@
         <v>305</v>
       </c>
       <c r="D246" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
@@ -4729,7 +4795,7 @@
         <v>305</v>
       </c>
       <c r="D247" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
@@ -4743,7 +4809,7 @@
         <v>305</v>
       </c>
       <c r="D248" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
@@ -4757,7 +4823,7 @@
         <v>305</v>
       </c>
       <c r="D249" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
@@ -4771,7 +4837,7 @@
         <v>305</v>
       </c>
       <c r="D250" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
@@ -4785,7 +4851,7 @@
         <v>305</v>
       </c>
       <c r="D251" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
@@ -4799,7 +4865,7 @@
         <v>305</v>
       </c>
       <c r="D252" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
@@ -4813,7 +4879,7 @@
         <v>305</v>
       </c>
       <c r="D253" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
@@ -4827,7 +4893,7 @@
         <v>305</v>
       </c>
       <c r="D254" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
@@ -4841,7 +4907,7 @@
         <v>305</v>
       </c>
       <c r="D255" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
@@ -4855,7 +4921,7 @@
         <v>305</v>
       </c>
       <c r="D256" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
@@ -4869,7 +4935,7 @@
         <v>305</v>
       </c>
       <c r="D257" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
@@ -4883,7 +4949,7 @@
         <v>305</v>
       </c>
       <c r="D258" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
@@ -4897,7 +4963,7 @@
         <v>305</v>
       </c>
       <c r="D259" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
@@ -4911,7 +4977,7 @@
         <v>305</v>
       </c>
       <c r="D260" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
@@ -4925,7 +4991,7 @@
         <v>305</v>
       </c>
       <c r="D261" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
@@ -4939,7 +5005,7 @@
         <v>305</v>
       </c>
       <c r="D262" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
@@ -4953,7 +5019,7 @@
         <v>305</v>
       </c>
       <c r="D263" t="s">
-        <v>305</v>
+        <v>326</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
@@ -4967,7 +5033,7 @@
         <v>305</v>
       </c>
       <c r="D264" t="s">
-        <v>305</v>
+        <v>327</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
@@ -4981,7 +5047,7 @@
         <v>305</v>
       </c>
       <c r="D265" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
@@ -4995,7 +5061,7 @@
         <v>305</v>
       </c>
       <c r="D266" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
@@ -5009,7 +5075,7 @@
         <v>305</v>
       </c>
       <c r="D267" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
@@ -5023,7 +5089,7 @@
         <v>305</v>
       </c>
       <c r="D268" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
@@ -5037,7 +5103,7 @@
         <v>305</v>
       </c>
       <c r="D269" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
@@ -5051,7 +5117,7 @@
         <v>305</v>
       </c>
       <c r="D270" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
@@ -5065,7 +5131,7 @@
         <v>305</v>
       </c>
       <c r="D271" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
@@ -5079,7 +5145,7 @@
         <v>305</v>
       </c>
       <c r="D272" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
@@ -5093,7 +5159,7 @@
         <v>305</v>
       </c>
       <c r="D273" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
@@ -5107,7 +5173,7 @@
         <v>305</v>
       </c>
       <c r="D274" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
@@ -5121,7 +5187,7 @@
         <v>305</v>
       </c>
       <c r="D275" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
@@ -5135,7 +5201,7 @@
         <v>305</v>
       </c>
       <c r="D276" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
@@ -5149,7 +5215,7 @@
         <v>305</v>
       </c>
       <c r="D277" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
@@ -5163,7 +5229,7 @@
         <v>305</v>
       </c>
       <c r="D278" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
@@ -5177,7 +5243,7 @@
         <v>305</v>
       </c>
       <c r="D279" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
@@ -5191,7 +5257,7 @@
         <v>305</v>
       </c>
       <c r="D280" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
@@ -5205,7 +5271,7 @@
         <v>305</v>
       </c>
       <c r="D281" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
@@ -5219,7 +5285,7 @@
         <v>305</v>
       </c>
       <c r="D282" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
@@ -5233,7 +5299,7 @@
         <v>305</v>
       </c>
       <c r="D283" t="s">
-        <v>305</v>
+        <v>324</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
@@ -5247,7 +5313,7 @@
         <v>305</v>
       </c>
       <c r="D284" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
@@ -5261,7 +5327,7 @@
         <v>305</v>
       </c>
       <c r="D285" t="s">
-        <v>305</v>
+        <v>326</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
@@ -5275,7 +5341,7 @@
         <v>305</v>
       </c>
       <c r="D286" t="s">
-        <v>305</v>
+        <v>327</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
@@ -5289,7 +5355,7 @@
         <v>305</v>
       </c>
       <c r="D287" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
@@ -5303,7 +5369,7 @@
         <v>305</v>
       </c>
       <c r="D288" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
@@ -5317,7 +5383,7 @@
         <v>305</v>
       </c>
       <c r="D289" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
@@ -5331,7 +5397,7 @@
         <v>305</v>
       </c>
       <c r="D290" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
@@ -5345,7 +5411,7 @@
         <v>305</v>
       </c>
       <c r="D291" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
@@ -5359,7 +5425,7 @@
         <v>305</v>
       </c>
       <c r="D292" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
@@ -5373,7 +5439,7 @@
         <v>305</v>
       </c>
       <c r="D293" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
@@ -5387,7 +5453,7 @@
         <v>305</v>
       </c>
       <c r="D294" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
@@ -5401,7 +5467,7 @@
         <v>305</v>
       </c>
       <c r="D295" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
@@ -5415,7 +5481,7 @@
         <v>305</v>
       </c>
       <c r="D296" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
@@ -5429,7 +5495,7 @@
         <v>305</v>
       </c>
       <c r="D297" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
@@ -5443,7 +5509,7 @@
         <v>305</v>
       </c>
       <c r="D298" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
@@ -5457,7 +5523,7 @@
         <v>305</v>
       </c>
       <c r="D299" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
@@ -5471,7 +5537,7 @@
         <v>305</v>
       </c>
       <c r="D300" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>

</xml_diff>